<commit_message>
complete working code with perfect print preview
</commit_message>
<xml_diff>
--- a/sample_products.xlsx.xlsx
+++ b/sample_products.xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Routisync\label-printer\label-printer-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D976737-E86A-4C06-A793-85CA960C40D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471782BB-144E-478B-B05E-D8163B328059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>MySKU</t>
   </si>
@@ -63,7 +63,16 @@
     <t>"Water; Sugar; Orange"</t>
   </si>
   <si>
-    <t>D:\Routisync\rsynclogo.png</t>
+    <t>SKU002</t>
+  </si>
+  <si>
+    <t>Apple Juice</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Banana"</t>
+  </si>
+  <si>
+    <t>D:\Routisync\logo.png</t>
   </si>
 </sst>
 </file>
@@ -382,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -394,7 +403,7 @@
     <col min="4" max="4" width="13.7265625" customWidth="1"/>
     <col min="5" max="5" width="16.453125" customWidth="1"/>
     <col min="6" max="6" width="14.81640625" customWidth="1"/>
-    <col min="8" max="8" width="27.7265625" customWidth="1"/>
+    <col min="8" max="8" width="34.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -452,7 +461,36 @@
         <v>8901234567890</v>
       </c>
       <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45987</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45988</v>
+      </c>
+      <c r="E3" s="1">
+        <v>46157</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>9.5</v>
+      </c>
+      <c r="H3">
+        <v>8901234567891</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete working and testing code with new FE code
</commit_message>
<xml_diff>
--- a/sample_products.xlsx.xlsx
+++ b/sample_products.xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Routisync\label-printer\label-printer-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471782BB-144E-478B-B05E-D8163B328059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855FD587-2525-4889-8B64-56C81515712E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,44 +25,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
-  <si>
-    <t>MySKU</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>MadeOn</t>
-  </si>
-  <si>
-    <t>PackedOn</t>
-  </si>
-  <si>
-    <t>UseBy</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>IngredientsList</t>
   </si>
   <si>
-    <t>MRP</t>
-  </si>
-  <si>
     <t>BarCode</t>
   </si>
   <si>
-    <t>LogoFile</t>
-  </si>
-  <si>
     <t>SKU001</t>
   </si>
   <si>
     <t>Orange Juice</t>
   </si>
   <si>
-    <t>"Water; Sugar; Orange"</t>
-  </si>
-  <si>
     <t>SKU002</t>
   </si>
   <si>
@@ -72,7 +48,175 @@
     <t>"Milk; Sugar; Banana"</t>
   </si>
   <si>
-    <t>D:\Routisync\logo.png</t>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>manufacturedDate</t>
+  </si>
+  <si>
+    <t>packagedDate</t>
+  </si>
+  <si>
+    <t>expiryDate</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
+    <t>Banana Juice</t>
+  </si>
+  <si>
+    <t>"Water; Sugar; Apple"</t>
+  </si>
+  <si>
+    <t>productImage</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Orange"</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\appleJuice.JPG</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\bananaJuice.JPEG</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\OrangeJuice.JPEG</t>
+  </si>
+  <si>
+    <t>Cherry juice</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Cherry"</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\Cherryjuice.JPG</t>
+  </si>
+  <si>
+    <t>Cranberry Juice</t>
+  </si>
+  <si>
+    <t>"Water; Sugar; Cranberry"</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\CranberryJuice.JPG</t>
+  </si>
+  <si>
+    <t>Grapefruit Juice</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Grapefruit"</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\GrapeJuice.JPG</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\GrapefruitJuice.JPG</t>
+  </si>
+  <si>
+    <t>Grape Juice</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Grape"</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\Lemonade_Juice.JPG</t>
+  </si>
+  <si>
+    <t>Lemonade Juice</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\MangoJuice.JPG</t>
+  </si>
+  <si>
+    <t>"Water; Sugar; Mango"</t>
+  </si>
+  <si>
+    <t>Mango Juice</t>
+  </si>
+  <si>
+    <t>Pineapple Juice</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\PineappleJuice.JPEG</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\PomegranateJuice.JPG</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Pineapple"</t>
+  </si>
+  <si>
+    <t>"Water; Sugar; Lemonade"</t>
+  </si>
+  <si>
+    <t>Pomegranate Juice</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Pomegranate"</t>
+  </si>
+  <si>
+    <t>Strawberry Juice</t>
+  </si>
+  <si>
+    <t>27/12/2025</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Strawberry"</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\StrawberryJuice.JPG</t>
+  </si>
+  <si>
+    <t>"Milk; Sugar; Kiwi"</t>
+  </si>
+  <si>
+    <t>KiwiJuice Juice</t>
+  </si>
+  <si>
+    <t>D:\Routisync\JuiceImages\KiwiJuice.JPEG</t>
+  </si>
+  <si>
+    <t>SKU003</t>
+  </si>
+  <si>
+    <t>SKU004</t>
+  </si>
+  <si>
+    <t>SKU005</t>
+  </si>
+  <si>
+    <t>SKU006</t>
+  </si>
+  <si>
+    <t>SKU007</t>
+  </si>
+  <si>
+    <t>SKU008</t>
+  </si>
+  <si>
+    <t>SKU009</t>
+  </si>
+  <si>
+    <t>SKU010</t>
+  </si>
+  <si>
+    <t>SKU011</t>
+  </si>
+  <si>
+    <t>SKU012</t>
+  </si>
+  <si>
+    <t>SKU013</t>
+  </si>
+  <si>
+    <t>D:\Routisync\label-printer\label-printer-dev\uploaded-images\logo.png</t>
   </si>
 </sst>
 </file>
@@ -108,9 +252,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -403,44 +550,49 @@
     <col min="4" max="4" width="13.7265625" customWidth="1"/>
     <col min="5" max="5" width="16.453125" customWidth="1"/>
     <col min="6" max="6" width="14.81640625" customWidth="1"/>
-    <col min="8" max="8" width="34.7265625" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.26953125" customWidth="1"/>
+    <col min="9" max="9" width="44.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>45976</v>
@@ -452,7 +604,7 @@
         <v>46157</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>12.5</v>
@@ -461,15 +613,18 @@
         <v>8901234567890</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1">
         <v>45987</v>
@@ -481,7 +636,7 @@
         <v>46157</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <v>9.5</v>
@@ -490,7 +645,362 @@
         <v>8901234567891</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45988</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45989</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45795</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4">
+        <v>11.5</v>
+      </c>
+      <c r="H4">
+        <v>8901234567891</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45986</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45987</v>
+      </c>
+      <c r="E5" s="1">
+        <v>46156</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5">
+        <v>14.5</v>
+      </c>
+      <c r="H5">
+        <v>8901234567881</v>
+      </c>
+      <c r="I5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45945</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45976</v>
+      </c>
+      <c r="E6" s="1">
+        <v>46280</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>89012345678921</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45987</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45988</v>
+      </c>
+      <c r="E7" s="1">
+        <v>46157</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7">
+        <v>9.5</v>
+      </c>
+      <c r="H7">
+        <v>8901237567891</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45988</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45989</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45795</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>11.5</v>
+      </c>
+      <c r="H8">
+        <v>8901234567891</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45955</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45987</v>
+      </c>
+      <c r="E9" s="1">
+        <v>46156</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9">
+        <v>14.5</v>
+      </c>
+      <c r="H9">
+        <v>8901234467881</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45973</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45976</v>
+      </c>
+      <c r="E10" s="1">
+        <v>46157</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10">
+        <v>12.5</v>
+      </c>
+      <c r="H10">
+        <v>8901234567890</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45956</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45973</v>
+      </c>
+      <c r="E11" s="1">
+        <v>46157</v>
+      </c>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11">
+        <v>9.5</v>
+      </c>
+      <c r="H11">
+        <v>8901234567891</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45988</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45989</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45795</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12">
+        <v>11.5</v>
+      </c>
+      <c r="H12">
+        <v>89012434567891</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45987</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="1">
+        <v>46156</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13">
+        <v>9.5</v>
+      </c>
+      <c r="H13">
+        <v>8901234567891</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45988</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45989</v>
+      </c>
+      <c r="E14" s="1">
+        <v>45795</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14">
+        <v>16.5</v>
+      </c>
+      <c r="H14">
+        <v>89012434567891</v>
+      </c>
+      <c r="I14" t="s">
+        <v>51</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>